<commit_message>
saveat rm from Scenarios
</commit_message>
<xml_diff>
--- a/cases/story_2/scenarios.xlsx
+++ b/cases/story_2/scenarios.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\HetaSimulator.jl\cases\story_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Julia\dev\HetaSimulator\cases\story_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30933698-427B-4FDD-B206-FD449A4281F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="conditions" sheetId="1" r:id="rId1"/>
@@ -20,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>saveat[]</t>
-  </si>
-  <si>
     <t>tspan</t>
   </si>
   <si>
@@ -35,9 +31,6 @@
   </si>
   <si>
     <t>dataone</t>
-  </si>
-  <si>
-    <t>0;12;24;48;72;120</t>
   </si>
   <si>
     <t>withdata2</t>
@@ -64,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -547,48 +540,48 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -865,31 +858,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -897,13 +890,10 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>1E-3</v>
@@ -911,27 +901,24 @@
       <c r="D2">
         <v>0.02</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2">
+      <c r="E2">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1E-3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>1E-3</v>
@@ -939,13 +926,13 @@
       <c r="C4">
         <v>0.1</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>1E-4</v>
@@ -953,11 +940,11 @@
       <c r="D5">
         <v>0.2</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>1000</v>
       </c>
-      <c r="G5" t="s">
-        <v>9</v>
+      <c r="F5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>